<commit_message>
Run after fixing the function by clipping between 0 and 1 the binary masks. The results got worse, and pretty bad. Needs more investigation
</commit_message>
<xml_diff>
--- a/src/Experiments.xlsx
+++ b/src/Experiments.xlsx
@@ -569,28 +569,28 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5511376545814535</v>
+        <v>0.00124669307300026</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7403166869671133</v>
+        <v>0.02086529610309911</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8548771955004575</v>
+        <v>0.1611430503889077</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7045908183632734</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8538366619441524</v>
+        <v>0.2860575767770462</v>
       </c>
       <c r="G2" t="n">
-        <v>0.06291125020060985</v>
+        <v>2.933411557641537e-05</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0446162832744569</v>
+        <v>0.03224457279426409</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -598,28 +598,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2770166704292962</v>
+        <v>0.03330472564329513</v>
       </c>
       <c r="C3" t="n">
-        <v>0.749134743630869</v>
+        <v>0.07755434396501001</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5712425534685374</v>
+        <v>0.1812411555871863</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4022656946556878</v>
+        <v>0.01104776235585715</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8892721924406496</v>
+        <v>0.3355435166647038</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2380018003620953</v>
+        <v>0.04398504287797503</v>
       </c>
       <c r="H3" t="n">
-        <v>0.448943738747438</v>
+        <v>0.1955116511847632</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5470769867967259</v>
+        <v>0.1838140241453101</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -627,28 +627,28 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3717049975084249</v>
+        <v>0.2157046534868357</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3894740039333905</v>
+        <v>0.08896976409543406</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4779058060185703</v>
+        <v>0.1775775833621003</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2696056453940782</v>
+        <v>0.0477085264313921</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8450031133250311</v>
+        <v>0.647393858279426</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2368120213530092</v>
+        <v>0.045964898724823</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5521571021571021</v>
+        <v>0.1284133973040299</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6985379550735864</v>
+        <v>0.3050628365290755</v>
       </c>
     </row>
   </sheetData>
@@ -701,28 +701,28 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7557743279060962</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03649503161698284</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.830672610290081</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7206170741273369</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8934377288345632</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02716164682076426</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -730,28 +730,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3215716297319097</v>
+        <v>0.004827801787229398</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0379577255135457</v>
+        <v>0.01212158443433304</v>
       </c>
       <c r="D3" t="n">
-        <v>0.209149692698</v>
+        <v>0.02105518643245047</v>
       </c>
       <c r="E3" t="n">
-        <v>0.41505897916437</v>
+        <v>8.471325169396249e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8879860708067324</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01125789193437968</v>
+        <v>0.000560878709978967</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0004398504508467121</v>
+        <v>1.379816594778222e-05</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2582184772128658</v>
+        <v>0.03588458870079315</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -759,28 +759,28 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7589911646586346</v>
+        <v>0.1567641988851329</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01632809873697354</v>
+        <v>0.04361828263447123</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2018331698072069</v>
+        <v>0.01883848451461288</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6334606205250597</v>
+        <v>0.02473802668608541</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5283704002569022</v>
+        <v>0.02280500569374648</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01401887457414732</v>
+        <v>0.0004942128287888125</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001001418676458316</v>
+        <v>0.008357239595376457</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4091542357654064</v>
+        <v>0.07988230396342109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>